<commit_message>
hettich csv & database.xlsx update
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61415\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61415\PycharmProjects\SlitherCabinet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23091E43-69AE-4B48-B843-F548F2F8FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644AE05E-E98D-4D63-BD35-3D1432A26EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5088EB7B-2BEC-4672-9A0E-B8F738A510D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -95,9 +95,6 @@
     <t>back jpeg (link to blob)</t>
   </si>
   <si>
-    <t>Manufacturer sku (xero product code)</t>
-  </si>
-  <si>
     <t>Manufacture Description (xero product name)</t>
   </si>
   <si>
@@ -152,14 +149,47 @@
     <t>Hardware type(ignore for now)</t>
   </si>
   <si>
-    <t>Supplier (Must be a contact (is supplier) in Xero, some type of check here)</t>
+    <t>Sales Unit</t>
+  </si>
+  <si>
+    <t>Delivery unit</t>
+  </si>
+  <si>
+    <t>ing</t>
+  </si>
+  <si>
+    <t>Hettich</t>
+  </si>
+  <si>
+    <t>Artia</t>
+  </si>
+  <si>
+    <t>Catalog Number from sample csv</t>
+  </si>
+  <si>
+    <t>Material Description from sample csv</t>
+  </si>
+  <si>
+    <t>Laminex</t>
+  </si>
+  <si>
+    <t>from sample csv</t>
+  </si>
+  <si>
+    <t>Manufacturer sku (LAMINEX + ' ' + Manufacturer sku = xero product code)</t>
+  </si>
+  <si>
+    <t>Manufacturer sku (HETTICH + ' ' + Manufacturer sku = xero product code)</t>
+  </si>
+  <si>
+    <t>Supplier, Must be a contact in Xero &amp; (IsSupplier=True), some type of check here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +197,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -275,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +327,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,11 +341,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,76 +680,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3859CCF1-7E3F-4F83-937C-07F2B7EC8E23}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="22" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
+      <c r="C1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="9"/>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -710,229 +775,215 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>31</v>
+      <c r="L3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="10"/>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J4" s="8"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="10"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J5" s="7" t="s">
+      <c r="L5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="10"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="J6" s="8"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="5"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L7" s="13"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="K10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G11" t="s">
         <v>12</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H11" t="s">
         <v>13</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I11" t="s">
         <v>14</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J11" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N11" t="s">
         <v>4</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O11" t="s">
         <v>5</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P11" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q11" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="R11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="11"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D12" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H12" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
         <v>2</v>
       </c>
-      <c r="G10" t="s">
+      <c r="K12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" t="s">
-        <v>8</v>
-      </c>
-      <c r="O10" t="s">
-        <v>8</v>
-      </c>
-      <c r="P10" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>3</v>
-      </c>
-      <c r="R10" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="R11" s="1"/>
-      <c r="S11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="2">
-        <v>16</v>
-      </c>
-      <c r="T12" s="2">
-        <v>18</v>
-      </c>
-      <c r="U12" s="2">
-        <v>25</v>
-      </c>
-      <c r="V12" s="2">
-        <v>32</v>
-      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="11"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="11"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M14" s="3"/>
@@ -940,22 +991,28 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="2" t="s">
+      <c r="R14" s="1"/>
+      <c r="S14" s="2">
+        <v>16</v>
+      </c>
+      <c r="T14" s="2">
+        <v>18</v>
+      </c>
+      <c r="U14" s="2">
         <v>25</v>
       </c>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
+      <c r="V14" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M15" s="3"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
@@ -963,40 +1020,67 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-    </row>
-    <row r="17" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-    </row>
-    <row r="18" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-    </row>
-    <row r="20" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="22" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="R10:R12"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="K8:M8"/>
+  <mergeCells count="5">
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="R11:V11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>